<commit_message>
finalize raw sequence dataset
</commit_message>
<xml_diff>
--- a/Project/data/full-sequences.xlsx
+++ b/Project/data/full-sequences.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zanebillings/Desktop/EPID-8200/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6D0C74-CA20-E440-8D5C-73D7DB5F56D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F04EE1-4C42-2149-8C5F-B0A014E0D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{901AA4D0-0F36-2041-AB50-36F3795354F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="163">
   <si>
     <t>Strain Name</t>
   </si>
@@ -1133,6 +1132,349 @@
 ACCGGTTCCAGATCAAGGGCGTTGAGCTGAAGTCAGGATACAAAGATTGGATCCTATGGATTTCCTTTGC
 CATATCATGTTTTTTGCTTTGTGTTGCTTTGTTGGGGTTCATCATGTGGGCCTGCCAAAAAGGCAACATT
 AGGTGCAACATTTGCATTTGA</t>
+  </si>
+  <si>
+    <t>A/H3N2/Perth/16/2009</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKLPGNDNSTATLCLGHHAVPNGTIVKTITNDQIEVTNATELVQSSSTGEICDSPHQILDGKNCTLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWTGVTQNGTSSACIRRSKNSFFSRLNWLTHLNFKYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQIFLYAQASGRITVSTKRSQQTVSPNIGSRPRVRNIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCNSECITPNGSIPNDKPFQNVNRITYGACPRYVKQNTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRLIGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGNGCFKIYHKCDNACIGSIRNGTYDHDVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNIRCNICI</t>
+  </si>
+  <si>
+    <t>GenBank: GQ293081.1</t>
+  </si>
+  <si>
+    <t>AAAGCAGGGGATAATTCTATTAACCATGAAGACTATCATTGCTTTGAGCTACATTCTATGTCTGGTTTTC
+GCTCAAAAACTTCCTGGAAATGACAACAGCACGGCAACGCTGTGCCTTGGGCACCATGCAGTACCAAACG
+GAACGATAGTGAAAACAATCACGAATGACCAAATTGAAGTTACTAATGCTACTGAGCTGGTTCAGAGTTC
+CTCAACAGGTGAAATATGCGACAGTCCTCATCAGATCCTTGATGGAAAAAACTGCACACTAATAGATGCT
+CTATTGGGAGACCCTCAGTGTGATGGCTTCCAAAATAAGAAATGGGACCTTTTTGTTGAACGCAGCAAAG
+CCTACAGCAACTGTTACCCTTATGATGTGCCGGATTATGCCTCCCTTAGGTCACTAGTTGCCTCATCCGG
+CACACTGGAGTTTAACAATGAAAGCTTCAATTGGACTGGAGTCACTCAAAACGGAACAAGCTCTGCTTGC
+ATAAGGAGATCTAAAAACAGTTTCTTTAGTAGATTGAATTGGTTGACCCACTTAAACTTCAAATACCCAG
+CATTGAACGTGACTATGCCAAACAATGAACAATTTGACAAATTGTACATTTGGGGGGTTCACCACCCGGG
+TACGGACAAAGACCAAATCTTCCTGTATGCTCAAGCATCAGGAAGAATCACAGTCTCTACCAAAAGAAGC
+CAACAAACCGTAAGCCCGAATATCGGATCTAGACCCAGAGTAAGGAATATCCCTAGCAGAATAAGCATCT
+ATTGGACAATAGTAAAACCGGGAGACATACTTTTGATTAACAGCACAGGGAATCTAATTGCTCCTAGGGG
+TTACTTCAAAATACGAAGTGGGAAAAGCTCAATAATGAGATCAGATGCACCCATTGGCAAATGCAATTCT
+GAATGCATCACTCCAAATGGAAGCATTCCCAATGACAAACCATTCCAAAATGTAAACAGGATCACATACG
+GGGCCTGTCCCAGATATGTTAAGCAAAACACTCTGAAATTGGCAACAGGGATGCGAAATGTACCAGAGAA
+ACAAACTAGAGGCATATTTGGCGCAATCGCGGGTTTCATAGAAAATGGTTGGGAGGGAATGGTGGATGGT
+TGGTACGGTTTCAGGCATCAAAATTCTGAGGGAAGAGGACAAGCAGCAGATCTCAAAAGCACTCAAGCAG
+CAATCGATCAAATCAATGGGAAGCTGAATAGATTGATCGGGAAAACCAACGAGAAATTCCATCAGATTGA
+AAAAGAATTCTCAGAAGTCGAAGGGAGAATTCAGGACCTTGAGAAATATGTTGAGGACACTAAAATAGAT
+CTCTGGTCATACAACGCGGAGCTTCTTGTTGCCCTGGAGAACCAACATACAATTGATCTAACTGACTCAG
+AAATGAACAAACTGTTTGAAAAAACAAAGAAGCAACTGAGGGAAAATGCTGAGGATATGGGCAATGGTTG
+TTTCAAAATATACCACAAATGTGACAATGCCTGCATAGGATCAATCAGAAATGGAACTTATGACCACGAT
+GTATACAGAGATGAAGCATTAAACAACCGGTTTCAGATCAAGGGAGTTGAGCTGAAGTCAGGGTACAAAG
+ATTGGATCCTATGGATTTCCTTTGCCATATCATGTTTTTTGCTTTGTGTTGCTTTGTTGGGGTTCATCAT
+GTGGGCCTGCCAAAAAGGCAACATTAGGTGCAACATTTGCATTTGAGTGCATTAATTAAAAACACCCTTG
+TTTCTAC</t>
+  </si>
+  <si>
+    <t>A/H3N2/Victoria/361/2011</t>
+  </si>
+  <si>
+    <t>MKTIIALSHILCLVFAQKLPGNDNSTATLCLGHHAVPNGTIVKTITNDQIEVTNATELVQNSSIGEICDSPHQILDGENCTLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWTGVTQNGTSSACIRRSNNSFFSRLNWLTHLNFKYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQIFLYAQSSGRITVSTKRSQQAVIPNIGSRPRIRNIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCNSECITPNGSIPNDKPFQNVNRITYGACPRYVKQSTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRLIGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGNGCFKIYHKCDNACIGSIRNGTYDHDVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNIRCNICI</t>
+  </si>
+  <si>
+    <t>GenBank: KM821347.1</t>
+  </si>
+  <si>
+    <t>CATGAAGACTATCATTGCTTTGAGCCACATTCTATGTCTGGTTTTCGCTCAAAAACTTCCTGGAAATGAC
+AACAGCACGGCAACGCTGTGCCTTGGGCACCATGCAGTACCAAACGGAACGATAGTGAAAACAATCACGA
+ATGACCAAATTGAAGTTACTAATGCTACTGAGCTGGTTCAGAATTCCTCAATAGGTGAAATATGCGACAG
+TCCTCATCAGATCCTTGATGGAGAAAACTGCACACTAATAGATGCTCTATTGGGAGACCCTCAGTGTGAT
+GGCTTCCAAAATAAGAAATGGGACCTTTTTGTTGAACGAAGCAAAGCCTACAGCAACTGTTACCCTTATG
+ATGTGCCGGATTATGCCTCCCTTAGGTCACTAGTTGCCTCATCCGGCACACTGGAGTTTAACAATGAAAG
+CTTCAATTGGACTGGAGTCACTCAAAACGGAACAAGTTCTGCTTGCATAAGGAGATCTAATAATAGTTTC
+TTTAGTAGATTAAATTGGTTGACCCACTTAAACTTCAAATACCCAGCATTGAACGTGACTATGCCAAACA
+ATGAACAATTTGACAAATTGTACATTTGGGGGGTTCACCACCCGGGTACGGACAAGGACCAAATCTTCCT
+GTATGCTCAATCATCAGGAAGAATCACAGTATCTACCAAAAGAAGCCAACAAGCTGTAATCCCGAATATC
+GGATCTAGACCCAGAATAAGGAATATCCCTAGCAGAATAAGCATCTATTGGACAATAGTAAAACCGGGAG
+ACATACTTTTGATTAACAGCACAGGGAATCTAATTGCTCCTAGGGGTTACTTCAAAATACGAAGTGGGAA
+AAGCTCAATAATGAGATCAGATGCACCCATTGGCAAATGCAATTCTGAATGCATCACTCCAAATGGAAGC
+ATTCCCAATGACAAACCATTCCAAAATGTAAACAGGATCACATACGGGGCCTGTCCCAGATATGTTAAGC
+AAAGCACTCTGAAATTGGCAACAGGAATGCGAAATGTACCAGAGAAACAAACTAGAGGCATATTTGGCGC
+AATAGCGGGTTTCATAGAAAATGGTTGGGAGGGAATGGTGGATGGTTGGTACGGTTTCAGGCATCAAAAT
+TCTGAGGGAAGAGGACAAGCAGCAGATCTCAAAAGCACTCAAGCAGCAATCGATCAAATCAATGGGAAGC
+TGAATCGATTGATCGGGAAAACCAACGAGAAATTCCATCAGATTGAAAAAGAATTCTCAGAAGTCGAAGG
+GAGAATTCAGGACCTTGAGAAATATGTTGAGGACACTAAAATAGATCTCTGGTCATACAACGCGGAGCTT
+CTTGTTGCCCTGGAGAACCAACATACAATTGATCTAACTGACTCAGAAATGAACAAACTGTTTGAAAAAA
+CAAAGAAGCAACTAAGGGAAAATGCTGAGGATATGGGCAATGGTTGTTTCAAAATATACCACAAATGTGA
+CAATGCCTGCATAGGATCAATCAGAAATGGAACTTATGACCACGATGTATACAGAGATGAAGCATTAAAC
+AACCGGTTCCAGATCAAGGGAGTTGAGCTGAAGTCAGGGTACAAAGATTGGATCCTATGGATTTCCTTTG
+CCATATCATGTTTTTTGCTTTGTGTTGCTTTGTTGGGGTTCATCATGTGGGCCTGCCAAAAGGGCAACAT
+TAGGTGCAACATTTGCATTTGAGTGCATTAATTAAAAACACCCTTGTTTCTACT</t>
+  </si>
+  <si>
+    <t>A/H3N2/Texas/50/2012</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKLPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGENCTLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWNGVTQNGTSSACIRRSNNSFFSRLNWLTHLNFKYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQIFLYAQPSGRITVSTKRSQQAVIPNIGSRPRIRNIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGACPRYVKQSTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRLIGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGNGCFKIYHKCDNACIGSIRNGTYDHDVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNIRCNICI</t>
+  </si>
+  <si>
+    <t>GenBank: KC892952.1</t>
+  </si>
+  <si>
+    <t>ATGAAGACTATCATTGCTTTGAGCTACATTCTATGTCTGGTTTTCGCTCAAAAACTTCCTGGAAATGACA
+ATAGCACGGCAACGCTGTGCCTTGGGCACCATGCAGTACCAAACGGAACGATAGTGAAAACAATCACGAA
+TGACCGAATTGAAGTTACTAATGCTACTGAACTGGTTCAGAATTCCTCAATAGGTGAAATATGCGACAGT
+CCTCATCAGATCCTTGATGGAGAAAACTGCACACTAATAGATGCTCTATTGGGAGACCCTCAGTGTGATG
+GCTTCCAAAATAAGAAATGGGACCTTTTTGTTGAACGAAGCAAAGCCTACAGCAACTGTTACCCTTATGA
+TGTGCCGGATTATGCCTCCCTTAGGTCACTAGTTGCCTCATCCGGCACACTGGAGTTTAACAATGAAAGC
+TTCAATTGGAATGGAGTCACTCAAAACGGAACAAGTTCTGCTTGCATAAGGAGATCTAATAATAGTTTCT
+TTAGTAGATTAAATTGGTTGACCCACTTAAACTTCAAATACCCAGCATTGAACGTGACTATGCCAAACAA
+TGAACAATTTGACAAATTGTACATTTGGGGGGTTCACCACCCGGGTACGGACAAGGACCAAATCTTCCTG
+TATGCTCAACCATCAGGAAGAATCACAGTATCTACCAAAAGAAGCCAACAAGCTGTAATCCCGAATATCG
+GATCTAGACCCAGAATAAGGAATATCCCTAGCAGAATAAGCATCTATTGGACAATAGTAAAACCGGGAGA
+CATACTTTTGATTAACAGCACAGGGAATCTAATTGCTCCTAGGGGTTACTTCAAAATACGAAGTGGGAAA
+AGCTCAATAATGAGATCAGATGCACCCATTGGCAAATGCAAGTCTGAATGCATCACTCCAAATGGAAGCA
+TTCCCAATGACAAACCATTCCAAAATGTAAACAGGATCACATACGGGGCCTGTCCCAGATATGTTAAGCA
+AAGCACTCTGAAATTGGCAACAGGAATGCGGAATGTACCAGAGAAACAAACTAGAGGCATATTTGGCGCA
+ATAGCGGGTTTCATAGAAAATGGTTGGGAGGGAATGGTGGATGGTTGGTACGGTTTCAGGCATCAAAATT
+CTGAGGGAAGAGGACAAGCAGCAGATCTCAAAAGCACTCAAGCAGCAATCGATCAAATCAATGGGAAGCT
+GAATCGATTGATCGGGAAAACCAACGAGAAATTCCATCAGATTGAAAAAGAATTCTCAGAAGTAGAAGGG
+AGAATTCAGGACCTTGAGAAATATGTTGAGGACACTAAAATAGATCTCTGGTCATACAACGCGGAGCTTC
+TTGTTGCCCTGGAGAACCAACATACAATTGATCTAACTGACTCAGAAATGAACAAACTGTTTGAAAAAAC
+AAAGAAGCAACTGAGGGAAAATGCTGAGGATATGGGCAATGGTTGTTTCAAAATATACCACAAATGTGAC
+AATGCCTGCATAGGATCAATCAGAAATGGAACTTATGACCACGATGTATACAGAGATGAAGCATTAAACA
+ACCGGTTCCAGATCAAGGGAGTTGAGCTGAAGTCAGGGTACAAAGATTGGATCCTATGGATTTCCTTTGC
+CATATCATGTTTTTTGCTTTGTGTTGCTTTGTTGGGGTTCATCATGTGGGCCTGCCAAAAGGGCAACATT
+AGGTGCAACATTTGCATTTGA</t>
+  </si>
+  <si>
+    <t>A/H3N2/Switzerland/9715293/2013</t>
+  </si>
+  <si>
+    <t>A/H3N2/Hong Kong/4801/2014</t>
+  </si>
+  <si>
+    <t>A/H3N2/Singapore/infimh-16-0019/2016</t>
+  </si>
+  <si>
+    <t>A/H3N2/Kansas/14/2017</t>
+  </si>
+  <si>
+    <t>MKTIIALSCILCLVFAQKIPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGENCTLIDALLGDPQCDGFQNKKWDLFVERNKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWAGVTQNGTSSSCIRGSKSSFFSRLNWLTHLNSKYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQISLYAQSSGRITVSTKRSQQAVIPNIGSRPRIRDIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGACPRYVKQSTLKLATGMRNVPERQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRLIGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGNGCFKIYHKCDNACMGSIRNGTYDHNVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNIRCNICI</t>
+  </si>
+  <si>
+    <t>GenBank: MG974450.1</t>
+  </si>
+  <si>
+    <t>GGATAATTCTATTAACCATGAAGACTATCATTGCTTTGAGCTGCATTCTATGTCTGGTTTTCGCTCAAAA
+AATTCCTGGAAATGACAATAGCACGGCAACGCTGTGCCTTGGGCACCATGCAGTACCAAACGGAACGATA
+GTGAAAACAATCACGAATGACCGAATTGAAGTTACTAATGCTACTGAGCTGGTTCAGAACTCCTCAATAG
+GTGAAATATGCGACAGTCCTCATCAGATCCTTGATGGAGAAAACTGCACACTAATAGATGCTCTATTGGG
+AGACCCTCAGTGTGATGGCTTTCAAAATAAGAAATGGGACCTTTTCGTTGAACGAAACAAAGCCTACAGC
+AACTGTTACCCTTATGATGTGCCGGATTATGCATCCCTTAGATCACTAGTTGCCTCATCCGGCACACTGG
+AGTTTAACAATGAAAGCTTCAATTGGGCTGGAGTCACTCAAAACGGAACAAGTTCTTCTTGCATAAGGGG
+ATCTAAAAGTAGTTTCTTTAGTAGATTAAATTGGTTGACCCACTTAAACTCCAAATACCCAGCATTAAAC
+GTGACTATGCCAAACAATGAACAATTTGACAAATTGTACATTTGGGGTGTTCACCACCCGGGTACGGACA
+AGGACCAAATCTCCCTGTATGCACAATCATCAGGAAGAATCACAGTATCTACCAAAAGAAGCCAACAAGC
+TGTAATCCCGAATATCGGATCTAGACCCAGAATAAGGGATATCCCTAGCAGAATAAGCATCTATTGGACA
+ATAGTAAAACCAGGAGACATACTTTTGATTAACAGCACAGGGAATCTAATTGCTCCTAGGGGTTACTTCA
+AAATACGAAGTGGGAAAAGCTCAATAATGAGATCAGATGCACCCATTGGCAAGTGCAAGTCTGAATGCAT
+CACTCCAAATGGAAGCATTCCAAATGACAAACCATTCCAAAATGTAAACAGGATCACATACGGGGCATGT
+CCCAGATATGTTAAGCAAAGCACTCTGAAATTGGCAACAGGAATGCGAAATGTACCAGAGAGACAAACTA
+GAGGCATATTTGGCGCAATAGCGGGTTTCATAGAAAATGGTTGGGAGGGAATGGTGGATGGTTGGTACGG
+CTTCAGGCATCAAAATTCTGAGGGAAGAGGACAAGCAGCAGATCTTAAAAGCACTCAAGCAGCAATCGAT
+CAAATCAATGGGAAGCTGAATCGATTGATCGGGAAAACCAACGAGAAATTCCATCAGATTGAAAAAGAGT
+TCTCAGAAGTAGAAGGGAGAATTCAGGACCTTGAGAAATATGTTGAGGACACAAAAATAGATCTCTGGTC
+ATACAACGCGGAGCTTCTTGTTGCCCTGGAGAACCAACATACAATTGATCTAACTGACTCAGAAATGAAC
+AAACTGTTTGAAAAAACAAAGAAGCAACTGAGGGAAAATGCTGAGGATATGGGCAATGGTTGTTTCAAAA
+TATACCACAAATGTGACAATGCCTGCATGGGGTCAATCAGAAATGGAACTTATGACCACAATGTATACAG
+GGATGAAGCATTAAACAACCGGTTCCAGATCAAGGGAGTTGAGCTGAAGTCAGGGTACAAAGATTGGATC
+CTATGGATTTCCTTTGCCATATCATGTTTTTTGCTTTGTGTTGCTCTGTTGGGGTTCATCATGTGGGCCT
+GCCAAAAGGGCAACATTAGGTGCAACATTTGCATTTGAGTGCATTAATTAAAAACAC</t>
+  </si>
+  <si>
+    <t>A/H3N2/South Australia/34/2019</t>
+  </si>
+  <si>
+    <t>ggataattctattaaccatgaagactatcattgctttgagctacattctatgtctggttttcgctcaaaaaattcctgga
+aatgacaatagcacggcaacgctgtgccttgggcaccatgcagtaccaaacggaacgatagtgaaaacaatcacaaatga
+ccgaattgaagttactaatgctactgagttggttcagaattcctcaataggtgaaatatgcgacagtcctcatcagatcc
+ttgatggagggaactgcacactaatagatgctctattgggggaccctcagtgtgacggctttcaaaataagaaatgggac
+ctttttgttgaacgaagcagagcctacagcaactgttacccttatgatgtaccggattatgcctcccttaggtcactagt
+tgcctcatccggcacactggagtttaaaaatgaaagcttcaattggactggagtcaaacaaaacggaacaagttctgctt
+gcataaggggatctagtagtagtttctttagtagattaaattggttgacccacttaaactacacatatccagcactgaac
+gtgactatgccaaacaaggaacaatttgacaaattgtacatttggggggttcaccacccgggtacggacaaggaccaaat
+cttcctgtatgctcaatcatcaggaagaatcacagtatctaccaaaagaagccaacaagctgtaatcccaaatatcggat
+ttagacccagaataagggatatccctagcagaataagcatctattggacaatagtaaaaccgggagacatacttttgatt
+aacagcacagggaatctaattgctcctaggggttacttcaaaatacgaagtgggaaaagctcaataatgagatcagatgc
+acccattggcaaatgcaagtctgaatgcatcactccaaatggaagcattcccaatgacaaaccattccaaaatgtaaaca
+ggatcacatacggggcctgtcccagatatgttaagcagagcactctgaaattggcaacaggaatgcgaaatgtaccagag
+aaacaaactagaggcatatttggcgcaatagcgggtttcatagaaaatggttgggagggaatgatggatggttggtacgg
+tttcaggcatcaaaattctgagggaagaggacaagcagcagatctcaaaagcactcaagcagcaatcgatcaaatcaatg
+ggaagctgaatcgattgatcggaaaaaccaacgagaaattccatcagatagaaaaagaattctcagaagtagaaggaaga
+gttcaagaccttgagaaatatgttgaggacactaaaatagatctctggtcatacaacgcggagcttcttgttgccctgga
+gaaccaacatacaattgacctaactgactcagaaatgaacaaactgtttgaaaaaacaaagaagcaactgagggaaaatg
+ctgaggatatgggaaatggttgtttcaaaatataccacaaatgtgacaatgcctgcataggatcaataagaaatgaaact
+tatgaccacaatgtgtacagggatgaagcattaaacaaccggttccagatcaagggagttgagctgaagtcagggtacaa
+agattggatcctatggatttcctttgccatatcatgttttttgctttgtattgctttgttggggttcatcatgtgggcct
+gccaaaagggcaacattagatgcaacatttgcatttgagtgcattaattaaaaac</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKIPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGGNC
+TLIDALLGDPQCDGFQNKKWDLFVERSRAYSNCYPYDVPDYASLRSLVASSGTLEFKNESFNWTGVKQNGTSSACIRGSS
+SSFFSRLNWLTHLNYTYPALNVTMPNKEQFDKLYIWGVHHPGTDKDQIFLYAQSSGRITVSTKRSQQAVIPNIGFRPRIR
+DIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGA
+CPRYVKQSTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMMDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRL
+IGKTNEKFHQIEKEFSEVEGRVQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGN
+GCFKIYHKCDNACIGSIRNETYDHNVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCIALLGFIMWACQKGNI
+RCNICI</t>
+  </si>
+  <si>
+    <t>Gisaid: EPI1387331</t>
+  </si>
+  <si>
+    <t>aaagcaggggatatttttattaaccatgaagactatcattgctttgagctacattctatgtctggttttcgctcaaaaaa
+ttcctggaaatgacaatagcacggcaacgctgtgccttgggcaccatgcagtaccaaacggaacgatagtgaaaacaatc
+acaaatgaccgaattgaagttactaatgctactgagttggttcagaattcctcaataggtgaaatatgcgacagtcctca
+tcagatccttgatggagagaactgcacactaatagatgctctattgggagaccctcagtgtgatggctttcaaaataaga
+aatgggacctttttgttgaacgaagcaaagcctacagcaactgttacccttatgatgtgccggattatgcctcccttagg
+tcactagttgcctcatccggcacactggagtttaaaaatgaaagcttcaattggactggagtcactcaaaacggaacaag
+ttctgcttgcataaggggatctagtagtagtttctttagtagattaaattggttgacccacttaaactacacatatccag
+cattgaacgtgactatgccaaacaaggaacaatttgacaaattgtacatttggggggttcaccacccgggtacggacaag
+gaccaaatcttcctgtatgctcaatcatcaggaagaatcacagtatctaccaaaagaagccaacaagctgtaatcccaaa
+tatcggatctagacccagaataagggatatccctagcagaataagcatctattggacaatagtaaaaccgggagacatac
+ttttgattaacagcacagggaatctaattgctcctaggggttacttcaaaatacgaagtgggaaaagctcaataatgaga
+tcagatgcacccattggcaaatgcaagtctgaatgcatcactccaaatggaagcattcccaatgacaaaccattccaaaa
+tgtaaacaggatcacatacggggcctgtcccagatatgttaagcatagcactctgaaattggcaacaggaatgcgaaatg
+taccagagaaacaaactagaggcatatttggcgcaatagcgggtttcatagaaaatggttgggagggaatggtggatggt
+tggtacggtttcaggcatcaaaattctgagggaagaggacaagcagcagatctcaaaagcactcaagcagcaatcgatca
+aatcaatgggaagctgaataggttgatcggaaaaaccaacgagaaattccatcagattgaaaaagaattctcagaagtag
+aaggaagagttcaagaccttgagaaatatgttgaggacactaaaatagatctctggtcatacaacgcggagcttcttgtt
+gccctggagaaccaacatacaattgatctaactgactcagaaatgaacaaactgtttgaaaaaacaaagaagcaactgag
+ggaaaatgctgaggatatgggaaatggttgtttcaaaatataccacaaatgtgacaatgcctgcatagaatcaataagaa
+atgaaacttatgaccacaatgtgtacagggatgaagcattgaacaaccggttccagatcaagggagttgagctgaagtca
+ggatacaaagattggatcctatggatttcctttgccatatcatgttttttgctttgtgttgctttgttggggttcatcat
+gtgggcctgccaaaagggcaacattagatgcaacatttgcatttgagtgcattaattaaaaacacccttgtttctact</t>
+  </si>
+  <si>
+    <t>Gisaid: EPI780183</t>
+  </si>
+  <si>
+    <t>Gisaid: EPI834581</t>
+  </si>
+  <si>
+    <t>Gisaid: EPI530687</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKIPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGENC
+TLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFKNESFNWTGVTQNGTSSACIRGSS
+SSFFSRLNWLTHLNYTYPALNVTMPNKEQFDKLYIWGVHHPGTDKDQIFLYAQSSGRITVSTKRSQQAVIPNIGSRPRIR
+DIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGA
+CPRYVKHSTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRL
+IGKTNEKFHQIEKEFSEVEGRVQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGN
+GCFKIYHKCDNACIESIRNETYDHNVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNI
+RCNICI</t>
+  </si>
+  <si>
+    <t>atgaagactatcattgctttgagctacattctatgtctggttttcgctcaaaaacttcctggaaatgacaatagcacggc
+aacgctgtgccttgggcaccatgcagtaccaaacggaacgatagtgaaaacaatcacgaatgaccgaattgaagttacta
+atgctactgagctggttcagaattcctcaataggtgaaatatgcgacagtcctcatcagatccttgatggagaaaactgc
+acactaatagatgctctattgggagaccctcagtgtgatggctttcaaaataagaaatgggacctttttgttgaacgaag
+caaagcctacagcaactgttacccttatgatgtgccggattatgcctcccttaggtcactagttgcctcatccggcacac
+tggagtttaacaatgaaagcttcaattgggctggagtcactcaaaacggaacaagttcttcttgcataaggggatctaat
+agtagtttctttagtagattaaattggttgacccacttaaactccaaatacccagcattaaacgtgactatgccaaacaa
+tgaacaatttgacaaattgtacatttggggggttcaccacccgggtacggacaaggaccaaatcttcctgtatgcacaat
+catcaggaagaatcacagtatctaccaaaagaagccaacaagctgtaatcccgaatatcggatctagacccagaataagg
+gatatccctagcagaataagcatctattggacaatagtaaaaccgggagacatacttttgattaacagcacagggaatct
+aattgctcctaggggttacttcaaaatacgaagtgggaaaagctcaataatgagatcagatgcacccattggcaaatgca
+agtctgaatgcatcactccaaatggaagcattcccaatgacaaaccattccaaaatgtaaacaggatcacatacggggcc
+tgtcccagatatgttaagcaaagcactctgaaattggcaacaggaatgcgaaatgtaccagagagacaaactagaggcat
+atttggcgcaatagcgggtttcatagaaaatggttgggagggaatggtggatggttggtacggcttcaggcatcaaaatt
+ctgagggaagaggacaagcagcagatctcaaaagcactcaagcagcaatcgatcaaatcaatgggaagctgaatcgattg
+atcgggaaaaccaacgagaaattccatcagattgaaaaagaattctcagaagtagaagggagaattcaggaccttgagaa
+atatgttgaggacacaaaaatagatctctggtcatacaacgcggagcttcttgttgccctggagaaccaacatacaattg
+atctaactgactcagaaatgaacaaactgtttgaaaaaacaaagaagcaactgagggaaaatgctgaggatatgggcaat
+ggttgtttcaaaatataccacaaatgtgacaatgcctgcataggatcaatcagaaatggaacttatgaccacgatgtata
+cagggatgaagcattaaacaaccggttccagatcaagggagttgagctgaagtcagggtacaaagattggatcctatgga
+tttcctttgccatatcatgttttttgctttgtgttgctttgttggggttcatcatgtgggcctgccaaaagggcaacatt
+aggtgcaacatttgcatttga</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKLPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGENC
+TLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWAGVTQNGTSSSCIRGSN
+SSFFSRLNWLTHLNSKYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQIFLYAQSSGRITVSTKRSQQAVIPNIGSRPRIR
+DIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGA
+CPRYVKQSTLKLATGMRNVPERQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRL
+IGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGN
+GCFKIYHKCDNACIGSIRNGTYDHDVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNI
+RCNICI</t>
+  </si>
+  <si>
+    <t>ggataattctattaaccatgaagactatcattgctttgagctacattctatgtctggttttcgctcaaaaaattcctgga
+aatgacaatagcacggcaacgctgtgccttgggcaccatgcagtaccaaacggaacgatagtgaaaacaatcacgaatga
+ccgaattgaagttactaatgctactgagctggttcagaattcctcaataggtgaaatatgcgacagtcctcatcagatcc
+ttgatggagaaaactgcacactaatagatgctctattgggagaccctcagtgtgatggctttcaaaataagaaatgggac
+ctttttgttgaacgaagcaaagcctacagcaactgttacccttatgatgtgccggattatgcctcccttaggtcactagt
+tgcctcatccggcacactggagtttaacaatgaaagcttcaattggactggagtcactcaaaacggaacaagttctgctt
+gcataaggagatctagtagtagtttctttagtagattaaattggttgacccacttaaactacacatacccagcattgaac
+gtgactatgccaaacaatgaacaatttgacaaattgtacatttggggggttcaccacccgggtacggacaaggaccaaat
+cttcctgtatgctcaatcatcaggaagaatcacagtatctaccaaaagaagccaacaagctgtaatcccaaatatcggat
+ctagacccagaataagggatatccctagcagaataagcatctattggacaatagtaaaaccgggagacatacttttgatt
+aacagcacagggaatctaattgctcctaggggttacttcaaaatacgaagtgggaaaagctcaataatgagatcagatgc
+acccattggcaaatgcaagtctgaatgcatcactccaaatggaagcattcccaatgacaaaccattccaaaatgtaaaca
+ggatcacatacggggcctgtcccagatatgttaagcatagcactctgaaattggcaacaggaatgcgaaatgtaccagag
+aaacaaactagaggcatatttggcgcaatagcgggtttcatagaaaatggttgggagggaatggtggatggttggtacgg
+tttcaggcatcaaaattctgagggaagaggacaagcagcagatctcaaaagcactcaagcagcaatcgatcaaatcaatg
+ggaagctgaatcgattgatcgggaaaaccaacgagaaattccatcagattgaaaaagaattctcagaagtagaaggaaga
+attcaggaccttgagaaatatgttgaggacactaaaatagatctctggtcatacaacgcggagcttcttgttgccctgga
+gaaccaacatacaattgatctaactgactcagaaatgaacaaactgtttgaaaaaacaaagaagcaactgagggaaaatg
+ctgaggatatgggcaatggttgtttcaaaatataccacaaatgtgacaatgcctgcataggatcaataagaaatggaact
+tatgaccacaatgtgtacagggatgaagcattaaacaaccggttccagatcaagggagttgagctgaagtcagggtacaa
+agattggatcctatggatttcctttgccatatcatgttttttgctttgtgttgctttgttggggttcatcatgtgggcct
+gccaaaagggcaacattaggtgcaacatttgcatttgagtgcattaattaaaaacac</t>
+  </si>
+  <si>
+    <t>MKTIIALSYILCLVFAQKIPGNDNSTATLCLGHHAVPNGTIVKTITNDRIEVTNATELVQNSSIGEICDSPHQILDGENC
+TLIDALLGDPQCDGFQNKKWDLFVERSKAYSNCYPYDVPDYASLRSLVASSGTLEFNNESFNWTGVTQNGTSSACIRRSS
+SSFFSRLNWLTHLNYTYPALNVTMPNNEQFDKLYIWGVHHPGTDKDQIFLYAQSSGRITVSTKRSQQAVIPNIGSRPRIR
+DIPSRISIYWTIVKPGDILLINSTGNLIAPRGYFKIRSGKSSIMRSDAPIGKCKSECITPNGSIPNDKPFQNVNRITYGA
+CPRYVKHSTLKLATGMRNVPEKQTRGIFGAIAGFIENGWEGMVDGWYGFRHQNSEGRGQAADLKSTQAAIDQINGKLNRL
+IGKTNEKFHQIEKEFSEVEGRIQDLEKYVEDTKIDLWSYNAELLVALENQHTIDLTDSEMNKLFEKTKKQLRENAEDMGN
+GCFKIYHKCDNACIGSIRNGTYDHNVYRDEALNNRFQIKGVELKSGYKDWILWISFAISCFLLCVALLGFIMWACQKGNI
+RCNICI</t>
+  </si>
+  <si>
+    <t>agcaaaagcaggggaaaataaaagcaacaaaaatgaaggcaatactagtagttctgctgtatacatttacaaccgcaaat
+gcagacacattatgtataggttatcatgcgaacaattcaacagacactgtagacacagtactagaaaagaatgtaacagt
+aacacactctgttaatcttctggaagacaagcataacggaaaactatgcaaactaggaggggtagccccattgcatttgg
+gtaaatgtaacattgctggctggatcctgggaaatccagagtgtgaatcactctccacagcaagatcatggtcctacatt
+gtggaaacatctaattcagacaatggaacgtgttacccaggagatttcatcaattatgaggagctaagagagcaattgag
+ctcagtgtcatcatttgaaaggtttgaaatattccccaagacaagttcatggcctaatcatgactcgaacaaaggtgtaa
+cggcagcatgtcctcacgctggagcaaaaagcttctacaaaaacttgatatggctggttaaaaaaggaaattcataccca
+aagctcaaccaaacctacattaatgataaagggaaagaagtcctcgtgctgtggggcattcaccatccacctactactgc
+tgaccaacaaagtctctatcagaatgcagatgcatatgtttttgtggggacatcaagatacagcaagaagttcaagccgg
+aaatagcaacaagacccaaagtgagggatcgagaagggagaatgaactattactggacactagtagagccgggagacaaa
+ataacattcgaagcaactggaaatctagtggtaccgagatatgcattcacaatggaaagaaatgctggatctggtattat
+catttcagatacgccagtccacgattgcaatacaacttgtcagacagccgagggtgctataaacaccagcctcccatttc
+agaatgtacatccggtcacaattgggaaatgtccaaagtatgtaaaaagcacaaaattgaggctggccacaggattgagg
+aatgtcccgtctattcaatctagaggcctattcggggccattgccggcttcattgaaggggggtggacagggatggtaga
+tggatggtacggttatcaccatcaaaatgagcaggggtcaggatatgcagccgatctgaagagcacacaaaatgccattg
+ataagattactaacaaagtaaattctgttattgaaaagatgaatacacagttcacagcagtgggtaaagagttcaaccac
+cttgaaaaaagaatagagaatctaaataaaaaagttgatgatggtttcctggacatttggacttacaatgccgaactgtt
+ggttctactggaaaatgaaagaactttggactatcacgattcaaatgtgaagaacttgtatgaaaaagtaagaaaccagt
+taaaaaacaatgccaaggaaattggaaacggctgctttgaattttaccacaaatgcgataacacatgcatggaaagtgtc
+aagaatgggacttatgactacccaaaatactcagaggaagcaaaattaaacagagaaaaaatagatggagtaaagctgga
+atcaacaaggatctaccagattttggcgatctattcaactgtcgccagttcattggtactggtagtctccctgggggcaa
+tcagcttctggatgtgctctaatgggtctctacaatgtagaatatgtatttaacattaggatttcagaatcatgagaaaa
+aacacccttgtttctact</t>
+  </si>
+  <si>
+    <t>MKAILVVLLYTFTTANADTLCIGYHANNSTDTVDTVLEKNVTVTHSVNLLEDKHNGKLCKLGGVAPLHLGKCNIAGWILG
+NPECESLSTARSWSYIVETSNSDNGTCYPGDFINYEELREQLSSVSSFERFEIFPKTSSWPNHDSNKGVTAACPHAGAKS
+FYKNLIWLVKKGNSYPKLNQTYINDKGKEVLVLWGIHHPPTTADQQSLYQNADAYVFVGTSRYSKKFKPEIATRPKVRDR
+EGRMNYYWTLVEPGDKITFEATGNLVVPRYAFTMERNAGSGIIISDTPVHDCNTTCQTAEGAINTSLPFQNVHPVTIGKC
+PKYVKSTKLRLATGLRNVPSIQSRGLFGAIAGFIEGGWTGMVDGWYGYHHQNEQGSGYAADLKSTQNAIDKITNKVNSVI
+EKMNTQFTAVGKEFNHLEKRIENLNKKVDDGFLDIWTYNAELLVLLENERTLDYHDSNVKNLYEKVRNQLKNNAKEIGNG
+CFEFYHKCDNTCMESVKNGTYDYPKYSEEAKLNREKIDGVKLESTRIYQILAIYSTVASSLVLVVSLGAISFWMCSNGSL
+QCRICI</t>
+  </si>
+  <si>
+    <t>Gisaid: EPI1415369</t>
   </si>
 </sst>
 </file>
@@ -1211,9 +1553,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1251,7 +1593,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1357,7 +1699,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1499,7 +1841,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1507,11 +1849,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6D73FA-7BE7-0543-958E-E8B52EDF41BD}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1827,9 +2169,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18">
+    <row r="19" spans="1:5" ht="409.6">
       <c r="A19" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="409.6">
@@ -2051,6 +2402,130 @@
       </c>
       <c r="E32" s="2" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="409.6">
+      <c r="A33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="409.6">
+      <c r="A34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="409.6">
+      <c r="A35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="409.6">
+      <c r="A36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="409.6">
+      <c r="A37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="409.6">
+      <c r="A38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="409.6">
+      <c r="A39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="409.6">
+      <c r="A40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start data processing script
</commit_message>
<xml_diff>
--- a/Project/data/full-sequences.xlsx
+++ b/Project/data/full-sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zanebillings/Desktop/EPID-8200/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F04EE1-4C42-2149-8C5F-B0A014E0D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CB5902-9E81-754F-8089-AEA6D8136B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{901AA4D0-0F36-2041-AB50-36F3795354F0}"/>
   </bookViews>
@@ -1481,7 +1481,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1490,21 +1490,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13.2"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="AtkinsonHyperlegible-Regular"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1527,14 +1515,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1852,330 +1838,333 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="16" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="16" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6">
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6">
+    <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.6">
+    <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6">
+    <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.6">
+    <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="409.6">
+    <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="409.6">
+    <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="409.6">
+    <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="409.6">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="409.6">
+    <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="409.6">
+    <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.6">
+    <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.6">
+    <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="409.6">
+    <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="409.6">
+    <row r="17" spans="1:5" ht="16" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="409.6">
+    <row r="18" spans="1:5" ht="16" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="409.6">
+    <row r="19" spans="1:5" ht="16" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>162</v>
       </c>
@@ -2183,285 +2172,286 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="409.6">
+    <row r="20" spans="1:5" ht="16" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="409.6">
+    <row r="21" spans="1:5" ht="16" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="409.6">
+    <row r="22" spans="1:5" ht="16" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="409.6">
+    <row r="23" spans="1:5" ht="16" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="409.6">
+    <row r="24" spans="1:5" ht="16" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="409.6">
+    <row r="25" spans="1:5" ht="16" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="409.6">
+    <row r="26" spans="1:5" ht="16" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="409.6">
+    <row r="27" spans="1:5" ht="16" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="409.6">
+    <row r="28" spans="1:5" ht="16" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="409.6">
+    <row r="29" spans="1:5" ht="16" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="409.6">
+    <row r="30" spans="1:5" ht="16" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="409.6">
+    <row r="31" spans="1:5" ht="16" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>122</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="409.6">
+    <row r="32" spans="1:5" ht="16" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="409.6">
+    <row r="33" spans="1:5" ht="16" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="409.6">
+    <row r="34" spans="1:5" ht="16" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="409.6">
+    <row r="35" spans="1:5" ht="16" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="409.6">
+    <row r="36" spans="1:5" ht="16" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>157</v>
       </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
         <v>154</v>
       </c>
@@ -2469,13 +2459,14 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="409.6">
+    <row r="37" spans="1:5" ht="16" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
         <v>153</v>
       </c>
@@ -2483,13 +2474,14 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="409.6">
+    <row r="38" spans="1:5" ht="16" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>155</v>
       </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
         <v>152</v>
       </c>
@@ -2497,30 +2489,31 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="409.6">
+    <row r="39" spans="1:5" ht="16" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="409.6">
+    <row r="40" spans="1:5" ht="16" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
feat: MSA and starts distance calculation
</commit_message>
<xml_diff>
--- a/Project/data/full-sequences.xlsx
+++ b/Project/data/full-sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zanebillings/Desktop/EPID-8200/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CB5902-9E81-754F-8089-AEA6D8136B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9008F1EF-F67E-B245-A222-70FFFCF6A77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{901AA4D0-0F36-2041-AB50-36F3795354F0}"/>
   </bookViews>
@@ -1481,7 +1481,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1493,6 +1493,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="AtkinsonHyperlegible-Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1515,12 +1521,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1835,11 +1842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6D73FA-7BE7-0543-958E-E8B52EDF41BD}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
@@ -1851,7 +1858,7 @@
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1">
+    <row r="1" spans="1:6" ht="16" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1867,8 +1874,9 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1884,8 +1892,9 @@
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1901,8 +1910,9 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1919,7 +1929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" spans="1:6" ht="16" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1936,7 +1946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1953,7 +1963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1970,7 +1980,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" spans="1:6" ht="16" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" spans="1:6" ht="16" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2004,7 +2014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -2021,7 +2031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
@@ -2038,7 +2048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2055,7 +2065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" spans="1:6" ht="16" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -2072,7 +2082,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" spans="1:6" ht="16" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2089,7 +2099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+    <row r="15" spans="1:6" ht="16" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" spans="1:6" ht="16" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>